<commit_message>
update report testcase doc
</commit_message>
<xml_diff>
--- a/testcases/template/报表.xlsx
+++ b/testcases/template/报表.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyCodes\sr_pro\starriver_pro_web\testcases\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21210" windowHeight="10800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24180" windowHeight="13050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="首页" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
+  <si>
+    <t>StarRiver 报表测试用例</t>
+  </si>
   <si>
     <t>测试结果</t>
   </si>
@@ -118,12 +121,33 @@
     <t>Bug#</t>
   </si>
   <si>
+    <t>report-statistics-001</t>
+  </si>
+  <si>
+    <t>统计:能耗</t>
+  </si>
+  <si>
+    <t>页面初始化</t>
+  </si>
+  <si>
+    <t>正常显示</t>
+  </si>
+  <si>
     <t>计数项:测试编号</t>
   </si>
   <si>
     <t>列标签</t>
   </si>
   <si>
+    <t>report-statistics-002</t>
+  </si>
+  <si>
+    <t>选择时间</t>
+  </si>
+  <si>
+    <t>选择开始时间，选择结束时间</t>
+  </si>
+  <si>
     <t>行标签</t>
   </si>
   <si>
@@ -133,65 +157,169 @@
     <t>总计</t>
   </si>
   <si>
-    <t>StarRiver 报表测试用例</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>report-statistics-001</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>report-statistics-002</t>
-  </si>
-  <si>
     <t>report-statistics-003</t>
   </si>
   <si>
+    <t>选择统计参数下拉框</t>
+  </si>
+  <si>
+    <t>显示 "按域” 和 "按设备“下拉列表</t>
+  </si>
+  <si>
     <t>report-statistics-004</t>
   </si>
   <si>
+    <t>选择统计参数：按域</t>
+  </si>
+  <si>
+    <t>域下拉框显示当前所有的可选域</t>
+  </si>
+  <si>
     <t>report-statistics-005</t>
   </si>
   <si>
+    <t>选择统计参数：按域：选择域</t>
+  </si>
+  <si>
+    <t>选中并显示所选域</t>
+  </si>
+  <si>
     <t>report-statistics-006</t>
   </si>
   <si>
+    <t>选择统计参数：按设备</t>
+  </si>
+  <si>
+    <t>显示选择设备输入框</t>
+  </si>
+  <si>
     <t>report-statistics-007</t>
   </si>
   <si>
+    <t>选择统计参数：按设备：选择设备面板</t>
+  </si>
+  <si>
+    <t>显示可选域下拉框，以及默认选中域的设备列表</t>
+  </si>
+  <si>
     <t>report-statistics-008</t>
   </si>
   <si>
+    <t>选择统计参数：按设备：选择设备面板：选择域</t>
+  </si>
+  <si>
+    <t>显示所选域的设备列表</t>
+  </si>
+  <si>
     <t>report-statistics-009</t>
   </si>
   <si>
+    <t>选择统计参数：按设备：选择设备面板：搜索设备</t>
+  </si>
+  <si>
+    <t>显示被搜索的设备</t>
+  </si>
+  <si>
     <t>report-statistics-010</t>
   </si>
   <si>
+    <t>选择统计参数：按设备：选择设备面板：设备列表分页</t>
+  </si>
+  <si>
+    <t>点击跳转至该分页设备列表</t>
+  </si>
+  <si>
     <t>report-statistics-011</t>
   </si>
   <si>
+    <t>选择统计参数：按设备：选择设备面板：选中设备</t>
+  </si>
+  <si>
+    <t>选中单一设备，设备输入框显示该设备</t>
+  </si>
+  <si>
     <t>report-statistics-012</t>
   </si>
   <si>
     <t>report-statistics-013</t>
   </si>
   <si>
+    <t>统计:照明</t>
+  </si>
+  <si>
     <t>report-statistics-014</t>
   </si>
   <si>
-    <t>统计:能耗</t>
-  </si>
-  <si>
-    <t>统计:能耗</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <t>选择域下拉框</t>
+  </si>
+  <si>
+    <t>显示可选域列表，</t>
+  </si>
+  <si>
+    <t>report-statistics-015</t>
+  </si>
+  <si>
+    <t>亮灯率统计面板</t>
+  </si>
+  <si>
+    <t>正确显示数据及亮灯率饼状图</t>
+  </si>
+  <si>
+    <t>report-statistics-016</t>
+  </si>
+  <si>
+    <t>故障率统计面板</t>
+  </si>
+  <si>
+    <t>正确显示数据及故障率饼状图</t>
+  </si>
+  <si>
+    <t>report-statistics-017</t>
+  </si>
+  <si>
+    <t>切换选中域</t>
+  </si>
+  <si>
+    <t>黄涛</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.0.2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加测试用例</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>report-statistics-018</t>
+  </si>
+  <si>
+    <t>点击应用，显示图表（数据为空）</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击应用，显示图表（有返回数据）</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据返回数据更新图表。</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>正常显示图表坐标</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据返回数据更新图表</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +351,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="8" tint="-0.249977111117893"/>
       <name val="等线"/>
@@ -244,25 +394,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="8" tint="-0.249977111117893"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -330,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -338,13 +471,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,26 +502,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -391,6 +524,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,7 +554,7 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor theme="0" tint="-0.14990691854609822"/>
         </patternFill>
       </fill>
     </dxf>
@@ -598,124 +735,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr lang="zh-CN" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="ctr"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="3"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr lang="zh-CN" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="ctr"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="4"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -733,7 +752,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Success</c:v>
+                  <c:v>(空白)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -809,148 +828,39 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>报表!$J$4:$J$6</c:f>
+              <c:f>报表!$J$4:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>(空白)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>统计:能耗</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>统计:照明</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>报表!$K$4:$K$6</c:f>
+              <c:f>报表!$K$4:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-072F-4FF0-B1B2-5230BD674595}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>报表!$L$2:$L$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>(空白)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr lang="zh-CN" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="zh-CN"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>报表!$J$4:$J$6</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>(空白)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>统计:能耗</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>报表!$L$4:$L$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="1">
-                  <c:v>13</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EEC4-4450-A17B-182858BB066B}"/>
+              <c16:uniqueId val="{00000000-F17E-4EA8-84AD-D1BCF7ED8016}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1779,12 +1689,12 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>13970</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>318770</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>814070</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1827,7 +1737,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="ccc" refreshedDate="43187.410750810188" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="65">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="ccc" refreshedDate="43192.345116550925" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="66">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="报表"/>
   </cacheSource>
@@ -1836,8 +1746,9 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="功能" numFmtId="0">
-      <sharedItems containsBlank="1" count="10">
+      <sharedItems containsBlank="1" count="11">
         <s v="统计:能耗"/>
+        <s v="统计:照明"/>
         <m/>
         <s v="文字属性" u="1"/>
         <s v="图片属性" u="1"/>
@@ -1850,17 +1761,17 @@
       </sharedItems>
     </cacheField>
     <cacheField name="测试目标/步骤" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="期望" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="测试结果" numFmtId="0">
-      <sharedItems containsBlank="1" count="4">
-        <s v="Success"/>
+      <sharedItems containsNonDate="0" containsBlank="1" count="4">
         <m/>
         <s v="Skip" u="1"/>
         <s v="Failed" u="1"/>
+        <s v="Success" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Bug#" numFmtId="0">
@@ -1876,525 +1787,533 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="65">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="66">
   <r>
     <s v="report-statistics-001"/>
     <x v="0"/>
-    <m/>
-    <m/>
+    <s v="页面初始化"/>
+    <s v="正常显示"/>
     <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="report-statistics-002"/>
     <x v="0"/>
-    <m/>
-    <m/>
+    <s v="选择时间"/>
+    <s v="选择开始时间，选择结束时间"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-003"/>
+    <x v="0"/>
+    <s v="选择统计参数下拉框"/>
+    <s v="显示 &quot;按域” 和 &quot;按设备“下拉列表"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-004"/>
+    <x v="0"/>
+    <s v="选择统计参数：按域"/>
+    <s v="域下拉框显示当前所有的可选域"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-005"/>
+    <x v="0"/>
+    <s v="选择统计参数：按域：选择域"/>
+    <s v="选中并显示所选域"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-006"/>
+    <x v="0"/>
+    <s v="选择统计参数：按设备"/>
+    <s v="显示选择设备输入框"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-007"/>
+    <x v="0"/>
+    <s v="选择统计参数：按设备：选择设备面板"/>
+    <s v="显示可选域下拉框，以及默认选中域的设备列表"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-008"/>
+    <x v="0"/>
+    <s v="选择统计参数：按设备：选择设备面板：选择域"/>
+    <s v="显示所选域的设备列表"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-009"/>
+    <x v="0"/>
+    <s v="选择统计参数：按设备：选择设备面板：搜索设备"/>
+    <s v="显示被搜索的设备"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-010"/>
+    <x v="0"/>
+    <s v="选择统计参数：按设备：选择设备面板：设备列表分页"/>
+    <s v="点击跳转至该分页设备列表"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-011"/>
+    <x v="0"/>
+    <s v="选择统计参数：按设备：选择设备面板：选中设备"/>
+    <s v="选中单一设备，设备输入框显示该设备"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-012"/>
+    <x v="0"/>
+    <s v="点击应用，显示图表（数据为空）"/>
+    <s v="正常显示图表坐标"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-013"/>
+    <x v="0"/>
+    <s v="点击应用，显示图表（有返回数据）"/>
+    <s v="根据返回数据更新图表。"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-014"/>
     <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-003"/>
-    <x v="0"/>
-    <m/>
-    <m/>
+    <s v="页面初始化"/>
+    <s v="正常显示"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-015"/>
     <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-004"/>
-    <x v="0"/>
-    <m/>
-    <m/>
+    <s v="选择域下拉框"/>
+    <s v="显示可选域列表，"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-016"/>
     <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-005"/>
-    <x v="0"/>
-    <m/>
-    <m/>
+    <s v="亮灯率统计面板"/>
+    <s v="正确显示数据及亮灯率饼状图"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-017"/>
     <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-006"/>
-    <x v="0"/>
-    <m/>
-    <m/>
+    <s v="故障率统计面板"/>
+    <s v="正确显示数据及故障率饼状图"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="report-statistics-018"/>
     <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-007"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-008"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-009"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-010"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-011"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-012"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-013"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="report-statistics-014"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="切换选中域"/>
+    <s v="根据返回数据更新图表（暂无API)"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <x v="0"/>
     <m/>
   </r>
 </pivotCacheRecords>
@@ -2402,21 +2321,22 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="J2:M6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="J2:L7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="11">
-        <item sd="0" m="1" x="2"/>
-        <item sd="0" x="1"/>
+      <items count="12">
         <item sd="0" m="1" x="3"/>
-        <item sd="0" m="1" x="5"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="8"/>
+        <item sd="0" x="2"/>
+        <item sd="0" m="1" x="4"/>
+        <item sd="0" m="1" x="6"/>
+        <item m="1" x="5"/>
         <item m="1" x="7"/>
         <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item m="1" x="10"/>
         <item x="0"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2424,10 +2344,10 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
       <items count="5">
+        <item m="1" x="2"/>
+        <item m="1" x="1"/>
         <item m="1" x="3"/>
-        <item m="1" x="2"/>
         <item x="0"/>
-        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2436,12 +2356,15 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="4">
     <i>
       <x v="1"/>
     </i>
     <i>
       <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
     </i>
     <i t="grand">
       <x/>
@@ -2450,10 +2373,7 @@
   <colFields count="1">
     <field x="4"/>
   </colFields>
-  <colItems count="3">
-    <i>
-      <x v="2"/>
-    </i>
+  <colItems count="2">
     <i>
       <x v="3"/>
     </i>
@@ -2464,7 +2384,7 @@
   <dataFields count="1">
     <dataField name="计数项:测试编号" fld="0" subtotal="count" baseField="1" baseItem="0"/>
   </dataFields>
-  <chartFormats count="5">
+  <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -2472,7 +2392,7 @@
             <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="0"/>
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -2484,7 +2404,7 @@
             <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="1"/>
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -2496,27 +2416,6 @@
             <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -2796,7 +2695,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2810,167 +2709,175 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
-      <c r="F1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="G1" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="I1" s="22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="13">
+      <c r="I2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="17">
         <v>43179</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="13">
+      <c r="I3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="17">
         <v>43182</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="D4" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="I4" s="16" t="s">
         <v>17</v>
       </c>
+      <c r="J4" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+      <c r="A5" s="12">
         <v>43187</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="D5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="I5" s="16" t="s">
         <v>22</v>
       </c>
+      <c r="J5" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
+      <c r="A6" s="12">
+        <v>43189</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="11"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2978,7 +2885,7 @@
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A3:D3"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -2986,27 +2893,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.375" customWidth="1"/>
     <col min="2" max="2" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="45.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.375" customWidth="1"/>
+    <col min="4" max="4" width="34.875" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="11.25" customWidth="1"/>
     <col min="7" max="7" width="18.375" customWidth="1"/>
     <col min="8" max="9" width="4" customWidth="1"/>
     <col min="10" max="10" width="15.625"/>
-    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.375"/>
+    <col min="11" max="11" width="9.125" customWidth="1"/>
+    <col min="12" max="12" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.125"/>
     <col min="16" max="16" width="10.875" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
@@ -3016,522 +2923,612 @@
     <col min="21" max="21" width="5.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="9">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="L5" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="J3" s="18" t="s">
+      <c r="J6" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="9">
+        <v>5</v>
+      </c>
+      <c r="L6" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="9">
+        <v>18</v>
+      </c>
+      <c r="L7" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M3" t="s">
+      <c r="D15" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="J4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="J5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" s="19">
-        <v>1</v>
-      </c>
-      <c r="L5" s="19">
-        <v>13</v>
-      </c>
-      <c r="M5" s="19">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="J6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="19">
-        <v>1</v>
-      </c>
-      <c r="L6" s="19">
-        <v>13</v>
-      </c>
-      <c r="M6" s="19">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
+      <c r="A23" s="2"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="7"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="A57" s="7"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="A59" s="7"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="A61" s="7"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="A65" s="7"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="7"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Skip"</formula>
@@ -3553,7 +3550,7 @@
           <x14:formula1>
             <xm:f>首页!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1532</xm:sqref>
+          <xm:sqref>E1:E1533</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>